<commit_message>
Added refined HGF for residues 305 to 470, updated the refinements spreadsheet, and began adding molprobity score outputs as pdf documents.
</commit_message>
<xml_diff>
--- a/Refinements.xlsx
+++ b/Refinements.xlsx
@@ -638,6 +638,10 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -646,10 +650,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="135">
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1142,27 +1142,27 @@
   <sheetData>
     <row r="1" spans="1:12" ht="46" customHeight="1">
       <c r="A1" s="3"/>
-      <c r="B1" s="35"/>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="32" t="s">
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="34"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="33" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2343,16 +2343,36 @@
       <c r="B33" s="18">
         <v>45</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="6"/>
+      <c r="C33" s="6">
+        <v>50.06</v>
+      </c>
+      <c r="D33" s="6">
+        <v>4</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6">
+        <v>2.79</v>
+      </c>
+      <c r="G33" s="6">
+        <v>32</v>
+      </c>
+      <c r="H33" s="6">
+        <v>4.32</v>
+      </c>
+      <c r="I33" s="6">
+        <v>96</v>
+      </c>
+      <c r="J33" s="7">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="K33" s="24">
+        <v>1.85</v>
+      </c>
+      <c r="L33" s="6">
+        <v>83</v>
+      </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="8" t="s">
@@ -3875,48 +3895,48 @@
         <v>77</v>
       </c>
       <c r="B74" s="30">
-        <f>AVERAGE(B3:B73)</f>
+        <f t="shared" ref="B74:G74" si="0">AVERAGE(B3:B73)</f>
         <v>63.89855072463768</v>
       </c>
       <c r="C74" s="30">
-        <f>AVERAGE(C3:C73)</f>
-        <v>43.10171428571428</v>
+        <f t="shared" si="0"/>
+        <v>43.199718309859144</v>
       </c>
       <c r="D74" s="30">
-        <f>AVERAGE(D3:D73)</f>
-        <v>31.357142857142858</v>
+        <f t="shared" si="0"/>
+        <v>30.971830985915492</v>
       </c>
       <c r="E74" s="31">
-        <f>AVERAGE(E3:E73)</f>
-        <v>2.7401428571428577E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.7015492957746485E-2</v>
       </c>
       <c r="F74" s="30">
-        <f>AVERAGE(F3:F73)</f>
-        <v>2.6507142857142858</v>
+        <f t="shared" si="0"/>
+        <v>2.6526760563380285</v>
       </c>
       <c r="G74" s="30">
-        <f>AVERAGE(G3:G73)</f>
-        <v>42.2</v>
+        <f t="shared" si="0"/>
+        <v>42.056338028169016</v>
       </c>
       <c r="H74" s="30">
-        <f t="shared" ref="H74:L74" si="0">AVERAGE(H3:H73)</f>
-        <v>1.5865714285714283</v>
+        <f t="shared" ref="H74:K74" si="1">AVERAGE(H3:H73)</f>
+        <v>1.6250704225352111</v>
       </c>
       <c r="I74" s="30">
-        <f t="shared" si="0"/>
-        <v>98.828571428571422</v>
+        <f t="shared" si="1"/>
+        <v>98.788732394366193</v>
       </c>
       <c r="J74" s="31">
         <f>AVERAGE(J3:J73)</f>
-        <v>2.0685714285714283E-3</v>
+        <v>2.1338028169014078E-3</v>
       </c>
       <c r="K74" s="30">
-        <f t="shared" si="0"/>
-        <v>1.401142857142857</v>
+        <f t="shared" si="1"/>
+        <v>1.4074647887323943</v>
       </c>
       <c r="L74" s="30">
         <f>AVERAGE(L3:L73)</f>
-        <v>95.057142857142864</v>
+        <v>94.887323943661968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>